<commit_message>
Updating Monocycle modules and testbench
</commit_message>
<xml_diff>
--- a/23InstructiosRISC32I.xlsx
+++ b/23InstructiosRISC32I.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Th25-J.B_F.C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD966AD4-5957-40FE-B4F9-4F1D8D2461CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803F405-4A37-4957-8102-C684BAEEA88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6428B508-3E23-4047-A819-2BA6D5444C44}"/>
   </bookViews>
@@ -746,22 +746,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -955,6 +939,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1040,17 +1040,17 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F6D51CA-DF14-404F-8A58-1F0198635215}" name="Tabla2" displayName="Tabla2" ref="B1:L25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D7463A58-C3CA-4F6C-8A47-A36A875CCCA8}" name="op" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{E1B20C18-0F27-446C-933D-81F1E86DB508}" name="funct3" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{A098A4CE-AE1F-4B95-8A7F-E598AFE8ED77}" name="funct7_5" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{0020EC18-F5DC-4D72-A1F5-E653E54B0736}" name="Instruct." dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{3477EF9C-022A-43B0-85EF-0FA6BA6E3B65}" name="RegWrite" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{DA634149-6F69-4E9E-93B6-4CB737EBE3E2}" name="ImmSrc" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9EBFEFE6-D2E4-4FD8-8552-3636AC7F8CEF}" name="ALUSrc" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{554D0BA3-C7EC-4080-BCD7-D3422A8B3D8D}" name="MemWrite" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{69A643AB-7CAD-461D-927A-0FAACED14321}" name="ResultSrc" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{413871B3-354B-40CC-9AC4-04478F0D39FD}" name="Branch" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{351A7E4D-1729-4921-B433-7A5D7F03448D}" name="ALUOp" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D7463A58-C3CA-4F6C-8A47-A36A875CCCA8}" name="op" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{E1B20C18-0F27-446C-933D-81F1E86DB508}" name="funct3" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{A098A4CE-AE1F-4B95-8A7F-E598AFE8ED77}" name="funct7_5" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0020EC18-F5DC-4D72-A1F5-E653E54B0736}" name="Instruct." dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3477EF9C-022A-43B0-85EF-0FA6BA6E3B65}" name="RegWrite" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DA634149-6F69-4E9E-93B6-4CB737EBE3E2}" name="ImmSrc" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9EBFEFE6-D2E4-4FD8-8552-3636AC7F8CEF}" name="ALUSrc" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{554D0BA3-C7EC-4080-BCD7-D3422A8B3D8D}" name="MemWrite" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{69A643AB-7CAD-461D-927A-0FAACED14321}" name="ResultSrc" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{413871B3-354B-40CC-9AC4-04478F0D39FD}" name="Branch" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{351A7E4D-1729-4921-B433-7A5D7F03448D}" name="ALUOp" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1377,7 +1377,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>